<commit_message>
Entire flow from invoice submission to view payment request done for po and support for multiple browsers added in test base
</commit_message>
<xml_diff>
--- a/src/main/java/com/billhub/qa/testdata/invoice_verification_sheet_po.xlsx
+++ b/src/main/java/com/billhub/qa/testdata/invoice_verification_sheet_po.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED199D5-BE71-40C3-B7AC-8EA11C19AFD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F672CED-A651-477E-A708-DD4D746912EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="336">
   <si>
     <t>Status</t>
   </si>
@@ -987,34 +987,46 @@
     <t>0</t>
   </si>
   <si>
+    <t>TESTINV45388</t>
+  </si>
+  <si>
+    <t>2024-03-15</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0.18</t>
+  </si>
+  <si>
+    <t>test_customer_1</t>
+  </si>
+  <si>
+    <t>test_comment_1</t>
+  </si>
+  <si>
+    <t>1.18</t>
+  </si>
+  <si>
+    <t>4500000888</t>
+  </si>
+  <si>
+    <t>1.00</t>
+  </si>
+  <si>
+    <t>test84</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>test</t>
   </si>
   <si>
-    <t>TESTINV45388</t>
-  </si>
-  <si>
-    <t>2024-03-15</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>0.18</t>
-  </si>
-  <si>
-    <t>test_customer_1</t>
-  </si>
-  <si>
-    <t>test_comment_1</t>
-  </si>
-  <si>
-    <t>1.18</t>
-  </si>
-  <si>
-    <t>4500000888</t>
-  </si>
-  <si>
-    <t>1.00</t>
+    <t>TESTINV90008</t>
+  </si>
+  <si>
+    <t>2024-03-13</t>
   </si>
 </sst>
 </file>
@@ -1221,25 +1233,25 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="left"/>
@@ -1597,7 +1609,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1669,16 +1681,16 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B2" s="53" t="s">
-        <v>323</v>
+        <v>334</v>
       </c>
       <c r="C2" s="54" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D2" s="55" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="56" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F2" s="57" t="s">
         <v>17</v>
@@ -1696,19 +1708,19 @@
         <v>18</v>
       </c>
       <c r="K2" s="62" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="L2" s="63" t="s">
         <v>65</v>
       </c>
       <c r="M2" s="64" t="s">
-        <v>322</v>
+        <v>333</v>
       </c>
       <c r="N2" t="s" s="0">
         <v>208</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>81</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -1825,16 +1837,16 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B2" s="38" t="s">
-        <v>323</v>
+        <v>334</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>324</v>
+        <v>335</v>
       </c>
       <c r="D2" s="40" t="s">
         <v>34</v>
       </c>
       <c r="E2" s="41" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F2" s="42" t="s">
         <v>321</v>
@@ -1846,25 +1858,25 @@
         <v>321</v>
       </c>
       <c r="I2" s="45" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="J2" s="46" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="K2" s="47" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="L2" s="48" t="s">
         <v>18</v>
       </c>
       <c r="M2" s="49" t="s">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="N2" s="50" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="O2" s="51" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="P2" s="52" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
All tests for invoice verification with excel sheet for Po based invoice added
</commit_message>
<xml_diff>
--- a/src/main/java/com/billhub/qa/testdata/invoice_verification_sheet_po.xlsx
+++ b/src/main/java/com/billhub/qa/testdata/invoice_verification_sheet_po.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="345">
   <si>
     <t>Status</t>
   </si>
@@ -1027,6 +1027,33 @@
   </si>
   <si>
     <t>2024-03-13</t>
+  </si>
+  <si>
+    <t>TESTINV74156</t>
+  </si>
+  <si>
+    <t>2024-03-28</t>
+  </si>
+  <si>
+    <t>test_customer_2</t>
+  </si>
+  <si>
+    <t>test_comment_2</t>
+  </si>
+  <si>
+    <t>4500000904</t>
+  </si>
+  <si>
+    <t>TESTINV85724</t>
+  </si>
+  <si>
+    <t>TESTINV71161</t>
+  </si>
+  <si>
+    <t>4.0</t>
+  </si>
+  <si>
+    <t>4.00</t>
   </si>
 </sst>
 </file>
@@ -1102,7 +1129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="416">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1252,6 +1279,1059 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="left"/>
@@ -1680,40 +2760,40 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B2" s="53" t="s">
-        <v>334</v>
-      </c>
-      <c r="C2" s="54" t="s">
-        <v>329</v>
-      </c>
-      <c r="D2" s="55" t="s">
+      <c r="B2" s="404" t="s">
+        <v>342</v>
+      </c>
+      <c r="C2" s="405" t="s">
+        <v>340</v>
+      </c>
+      <c r="D2" s="406" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="56" t="s">
-        <v>330</v>
-      </c>
-      <c r="F2" s="57" t="s">
+      <c r="E2" s="407" t="s">
+        <v>344</v>
+      </c>
+      <c r="F2" s="408" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="58" t="s">
+      <c r="G2" s="409" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="59" t="s">
+      <c r="H2" s="410" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="60" t="s">
+      <c r="I2" s="411" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="61" t="s">
+      <c r="J2" s="412" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="62" t="s">
+      <c r="K2" s="413" t="s">
         <v>85</v>
       </c>
-      <c r="L2" s="63" t="s">
+      <c r="L2" s="414" t="s">
         <v>65</v>
       </c>
-      <c r="M2" s="64" t="s">
+      <c r="M2" s="415" t="s">
         <v>333</v>
       </c>
       <c r="N2" t="s" s="0">
@@ -1836,49 +2916,49 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B2" s="38" t="s">
-        <v>334</v>
-      </c>
-      <c r="C2" s="39" t="s">
-        <v>335</v>
-      </c>
-      <c r="D2" s="40" t="s">
+      <c r="B2" s="389" t="s">
+        <v>342</v>
+      </c>
+      <c r="C2" s="390" t="s">
+        <v>337</v>
+      </c>
+      <c r="D2" s="391" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="41" t="s">
-        <v>324</v>
-      </c>
-      <c r="F2" s="42" t="s">
+      <c r="E2" s="392" t="s">
+        <v>343</v>
+      </c>
+      <c r="F2" s="393" t="s">
         <v>321</v>
       </c>
-      <c r="G2" s="43" t="s">
+      <c r="G2" s="394" t="s">
         <v>321</v>
       </c>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="395" t="s">
         <v>321</v>
       </c>
-      <c r="I2" s="45" t="s">
+      <c r="I2" s="396" t="s">
         <v>321</v>
       </c>
-      <c r="J2" s="46" t="s">
+      <c r="J2" s="397" t="s">
         <v>321</v>
       </c>
-      <c r="K2" s="47" t="s">
+      <c r="K2" s="398" t="s">
         <v>321</v>
       </c>
-      <c r="L2" s="48" t="s">
+      <c r="L2" s="399" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="49" t="s">
-        <v>333</v>
-      </c>
-      <c r="N2" s="50" t="s">
-        <v>333</v>
-      </c>
-      <c r="O2" s="51" t="s">
-        <v>324</v>
-      </c>
-      <c r="P2" s="52" t="s">
+      <c r="M2" s="400" t="s">
+        <v>326</v>
+      </c>
+      <c r="N2" s="401" t="s">
+        <v>327</v>
+      </c>
+      <c r="O2" s="402" t="s">
+        <v>343</v>
+      </c>
+      <c r="P2" s="403" t="s">
         <v>19</v>
       </c>
       <c r="Q2" t="s" s="0">

</xml_diff>